<commit_message>
Revert "Normalized line endings"
This reverts commit 7dd5b7794ce8da8b81a2899953701ea87cc474c3.
</commit_message>
<xml_diff>
--- a/app/config/tables/Ethiopia_members/forms/Ethiopia_Section3/Ethiopia_Section3.xlsx
+++ b/app/config/tables/Ethiopia_members/forms/Ethiopia_Section3/Ethiopia_Section3.xlsx
@@ -1,3 +1,26 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <bookViews>
+    <workbookView xWindow="420" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+  </bookViews>
+  <sheets>
+    <sheet name="initial" sheetId="5" r:id="rId1"/>
+    <sheet name="survey" sheetId="1" r:id="rId2"/>
+    <sheet name="choices" sheetId="2" r:id="rId3"/>
+    <sheet name="settings" sheetId="3" r:id="rId4"/>
+    <sheet name="model" sheetId="4" r:id="rId5"/>
+  </sheets>
+  <calcPr calcId="140000" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
+</workbook>
+</file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="154">
@@ -1089,6 +1112,491 @@
 </a:theme>
 </file>
 
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3" s="29" customFormat="1">
+      <c r="A1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="21" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="29.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="30" customFormat="1">
+      <c r="A1" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30">
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30">
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="31" customFormat="1" ht="30">
+      <c r="B4" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="31" customFormat="1" ht="45">
+      <c r="D5" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="32" customFormat="1" ht="75">
+      <c r="A6" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="32" customFormat="1" ht="30">
+      <c r="D7" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="32" customFormat="1">
+      <c r="D8" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="33" customFormat="1" ht="30">
+      <c r="B9" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="33" customFormat="1">
+      <c r="D10" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="33" customFormat="1"/>
+    <row r="12" spans="1:7" s="33" customFormat="1" ht="75">
+      <c r="A12" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="33" customFormat="1"/>
+    <row r="14" spans="1:7" s="33" customFormat="1">
+      <c r="B14" s="33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="32" customFormat="1">
+      <c r="B15" s="32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="31" customFormat="1" ht="30">
+      <c r="D16" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="31" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" s="31" customFormat="1">
+      <c r="B17" s="31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="29" customFormat="1">
+      <c r="A1" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="34" customFormat="1">
+      <c r="A2" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="34" customFormat="1">
+      <c r="A3" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="35" customFormat="1">
+      <c r="A4" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="35" customFormat="1">
+      <c r="A5" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="35" customFormat="1">
+      <c r="A6" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="36" customFormat="1">
+      <c r="A7" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="36" customFormat="1">
+      <c r="A8" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="36" customFormat="1">
+      <c r="A9" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="36" customFormat="1">
+      <c r="A10" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="37" customFormat="1">
+      <c r="A11" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="37" customFormat="1">
+      <c r="A12" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="37" customFormat="1">
+      <c r="A13" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="29" customFormat="1">
+      <c r="A1" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C64"/>

</xml_diff>